<commit_message>
cập nhật báo cáo cdvt
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/CDVT/thoatnuoc.xlsx
+++ b/QUANGHANH2/excel/CDVT/thoatnuoc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONG\Desktop\QUANGHANH-PROTOTYPE\QUANGHANH2\excel\CDVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONG\Desktop\QUANGHANH-PROTOTYPE-master\QUANGHANH2\excel\CDVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC25A112-D1F5-4066-A3B1-3208A0F745E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F723861-A766-4F1C-9E23-7E69AC01ED0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="12915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,13 +395,14 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>

</xml_diff>